<commit_message>
commiting for user testing
</commit_message>
<xml_diff>
--- a/Documentation/WebDevProject_userStories.xlsx
+++ b/Documentation/WebDevProject_userStories.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Owner/Desktop/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Owner/Desktop/WebDevProject-zrobinso/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E25E9C9-474F-B545-B67D-F4DCB8757B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F731BCD3-69E5-A54A-A612-1D5FEFE4BEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26680" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>So that I get credit for my work</t>
-  </si>
-  <si>
-    <t>I want to find key information on field trsips, city tours, the Incline’s history, visitor details, and gift shop products.</t>
   </si>
   <si>
     <r>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t>I want to see the same colors, font size, and font logo consistancy used across all media</t>
+  </si>
+  <si>
+    <t>I want to find key information on field trips, city tours, the Incline’s history, visitor details, and gift shop products.</t>
   </si>
 </sst>
 </file>
@@ -1529,7 +1529,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1572,7 +1572,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>21</v>
@@ -1614,10 +1614,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1628,7 +1628,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>18</v>

</xml_diff>